<commit_message>
fixing error in log
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PVsO8R9L</t>
+          <t>JdCcx1nT</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Uw8wpQeH</t>
+          <t>Ha1VYKm9</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>cuVTaRsm</t>
+          <t>W3OWoMfa</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some error in send sms whit kavenegar
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p30-1\Desktop\pythonProject\creat-user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9882166-32FC-47D7-B2BC-1C3563965816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1CFF1C-B73A-411B-967C-DDF509F70F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="4215" windowWidth="24300" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
     <t>lastName</t>
   </si>
   <si>
+    <t>phone</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -46,7 +49,7 @@
     <t>example6@gmail.com</t>
   </si>
   <si>
-    <t>D17xXVVw</t>
+    <t>4kTWgnoA</t>
   </si>
   <si>
     <t>مهدي</t>
@@ -58,10 +61,7 @@
     <t>example2@gmail.com</t>
   </si>
   <si>
-    <t>quMjzom1</t>
-  </si>
-  <si>
-    <t>phone</t>
+    <t>7Ab1160p</t>
   </si>
 </sst>
 </file>
@@ -427,12 +427,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -446,13 +447,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,19 +461,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>9195182813</v>
+        <v>9381088235</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,19 +481,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>9306498871</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>